<commit_message>
shrinked png, edited text
</commit_message>
<xml_diff>
--- a/documentation/asciiunit/Bildschirm.xlsx
+++ b/documentation/asciiunit/Bildschirm.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>X</t>
   </si>
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -727,6 +727,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -763,21 +772,102 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1014,8 +1104,8 @@
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2011680" cy="657296"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Textfeld 1"/>
@@ -1154,7 +1244,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Textfeld 1"/>
@@ -1811,32 +1901,32 @@
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="42">
+      <c r="E5" s="51">
         <v>0</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="18"/>
       <c r="J5" s="26"/>
       <c r="K5" s="23"/>
       <c r="L5" s="18"/>
-      <c r="M5" s="51">
+      <c r="M5" s="60">
         <v>1</v>
       </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="53"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="62"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="33"/>
       <c r="S5" s="17"/>
       <c r="T5" s="23"/>
-      <c r="U5" s="51">
+      <c r="U5" s="60">
         <v>2</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="53"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="62"/>
       <c r="Y5" s="18"/>
       <c r="Z5" s="33"/>
       <c r="AA5" s="17"/>
@@ -1891,26 +1981,26 @@
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="18"/>
       <c r="J6" s="26"/>
       <c r="K6" s="23"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="56"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="65"/>
       <c r="Q6" s="18"/>
       <c r="R6" s="33"/>
       <c r="S6" s="17"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="55"/>
-      <c r="X6" s="56"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="65"/>
       <c r="Y6" s="18"/>
       <c r="Z6" s="33"/>
       <c r="AA6" s="17"/>
@@ -1965,26 +2055,26 @@
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="18"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="56"/>
       <c r="I7" s="18"/>
       <c r="J7" s="26"/>
       <c r="K7" s="23"/>
       <c r="L7" s="18"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="56"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="65"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="33"/>
       <c r="S7" s="17"/>
       <c r="T7" s="23"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="56"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="65"/>
       <c r="Y7" s="18"/>
       <c r="Z7" s="33"/>
       <c r="AA7" s="17"/>
@@ -2039,26 +2129,26 @@
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="18"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="50"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
       <c r="I8" s="18"/>
       <c r="J8" s="26"/>
       <c r="K8" s="23"/>
       <c r="L8" s="18"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="59"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="68"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="33"/>
       <c r="S8" s="17"/>
       <c r="T8" s="23"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="59"/>
+      <c r="U8" s="66"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="68"/>
       <c r="Y8" s="18"/>
       <c r="Z8" s="33"/>
       <c r="AA8" s="17"/>
@@ -2411,22 +2501,22 @@
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="61"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="18"/>
       <c r="J13" s="26"/>
       <c r="K13" s="23"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="51" t="s">
+      <c r="M13" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="44"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="33"/>
       <c r="S13" s="17"/>
@@ -2438,12 +2528,12 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="33"/>
       <c r="AA13" s="17"/>
-      <c r="AB13" s="68"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="61"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="43"/>
+      <c r="AF13" s="43"/>
+      <c r="AG13" s="44"/>
       <c r="AH13" s="33"/>
       <c r="AI13" s="17"/>
       <c r="AJ13" s="40"/>
@@ -2489,18 +2579,18 @@
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="64"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="18"/>
       <c r="J14" s="26"/>
       <c r="K14" s="23"/>
       <c r="L14" s="18"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="64"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="47"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="33"/>
       <c r="S14" s="17"/>
@@ -2512,12 +2602,12 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="33"/>
       <c r="AA14" s="17"/>
-      <c r="AB14" s="62"/>
-      <c r="AC14" s="63"/>
-      <c r="AD14" s="63"/>
-      <c r="AE14" s="63"/>
-      <c r="AF14" s="63"/>
-      <c r="AG14" s="64"/>
+      <c r="AB14" s="45"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="46"/>
+      <c r="AE14" s="46"/>
+      <c r="AF14" s="46"/>
+      <c r="AG14" s="47"/>
       <c r="AH14" s="33"/>
       <c r="AI14" s="17"/>
       <c r="AJ14" s="40"/>
@@ -2563,18 +2653,18 @@
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="64"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
       <c r="I15" s="18"/>
       <c r="J15" s="26"/>
       <c r="K15" s="23"/>
       <c r="L15" s="18"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="64"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="47"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="33"/>
       <c r="S15" s="17"/>
@@ -2586,12 +2676,12 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="33"/>
       <c r="AA15" s="17"/>
-      <c r="AB15" s="62"/>
-      <c r="AC15" s="63"/>
-      <c r="AD15" s="63"/>
-      <c r="AE15" s="63"/>
-      <c r="AF15" s="63"/>
-      <c r="AG15" s="64"/>
+      <c r="AB15" s="45"/>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="46"/>
+      <c r="AE15" s="46"/>
+      <c r="AF15" s="46"/>
+      <c r="AG15" s="47"/>
       <c r="AH15" s="33"/>
       <c r="AI15" s="17"/>
       <c r="AJ15" s="40"/>
@@ -2637,18 +2727,18 @@
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="18"/>
       <c r="J16" s="26"/>
       <c r="K16" s="23"/>
       <c r="L16" s="18"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="67"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="33"/>
       <c r="S16" s="17"/>
@@ -2660,12 +2750,12 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="33"/>
       <c r="AA16" s="17"/>
-      <c r="AB16" s="65"/>
-      <c r="AC16" s="66"/>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="66"/>
-      <c r="AG16" s="67"/>
+      <c r="AB16" s="48"/>
+      <c r="AC16" s="49"/>
+      <c r="AD16" s="49"/>
+      <c r="AE16" s="49"/>
+      <c r="AF16" s="49"/>
+      <c r="AG16" s="50"/>
       <c r="AH16" s="33"/>
       <c r="AI16" s="17"/>
       <c r="AJ16" s="40"/>
@@ -4515,8 +4605,8 @@
   </sheetPr>
   <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AL16" sqref="AL16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.77734375" defaultRowHeight="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4715,36 +4805,44 @@
         <v>1</v>
       </c>
       <c r="C4" s="23"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="D4" s="69">
+        <v>0</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="26"/>
       <c r="K4" s="23"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
+      <c r="L4" s="70">
+        <v>1</v>
+      </c>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="80"/>
       <c r="R4" s="33"/>
       <c r="S4" s="17"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
+      <c r="T4" s="70">
+        <v>2</v>
+      </c>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
       <c r="Z4" s="33"/>
       <c r="AA4" s="17"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
+      <c r="AB4" s="70">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="72"/>
       <c r="AH4" s="33"/>
       <c r="AI4" s="17"/>
       <c r="AJ4" s="40"/>
@@ -4755,42 +4853,36 @@
         <v>2</v>
       </c>
       <c r="C5" s="23"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="42">
-        <v>0</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="18"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="26"/>
       <c r="K5" s="23"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="51">
-        <v>1</v>
-      </c>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="18"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="83"/>
       <c r="R5" s="33"/>
       <c r="S5" s="17"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="51">
-        <v>2</v>
-      </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="18"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
       <c r="Z5" s="33"/>
       <c r="AA5" s="17"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
+      <c r="AB5" s="73"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74"/>
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="75"/>
       <c r="AH5" s="33"/>
       <c r="AI5" s="17"/>
       <c r="AJ5" s="40"/>
@@ -4801,36 +4893,36 @@
         <v>3</v>
       </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="18"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="26"/>
       <c r="K6" s="23"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="18"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="83"/>
       <c r="R6" s="33"/>
       <c r="S6" s="17"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="55"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="18"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="82"/>
+      <c r="Y6" s="83"/>
       <c r="Z6" s="33"/>
       <c r="AA6" s="17"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
+      <c r="AB6" s="73"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="74"/>
+      <c r="AF6" s="74"/>
+      <c r="AG6" s="75"/>
       <c r="AH6" s="33"/>
       <c r="AI6" s="17"/>
       <c r="AJ6" s="40"/>
@@ -4841,36 +4933,36 @@
         <v>4</v>
       </c>
       <c r="C7" s="23"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="46"/>
       <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="26"/>
       <c r="K7" s="23"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="18"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="83"/>
       <c r="R7" s="33"/>
       <c r="S7" s="17"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="56"/>
-      <c r="Y7" s="18"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="82"/>
+      <c r="W7" s="82"/>
+      <c r="X7" s="82"/>
+      <c r="Y7" s="83"/>
       <c r="Z7" s="33"/>
       <c r="AA7" s="17"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
+      <c r="AB7" s="73"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="75"/>
       <c r="AH7" s="33"/>
       <c r="AI7" s="17"/>
       <c r="AJ7" s="40"/>
@@ -4881,36 +4973,36 @@
         <v>5</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="18"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="26"/>
       <c r="K8" s="23"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="18"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="83"/>
       <c r="R8" s="33"/>
       <c r="S8" s="17"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="59"/>
-      <c r="Y8" s="18"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="82"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="83"/>
       <c r="Z8" s="33"/>
       <c r="AA8" s="17"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="75"/>
       <c r="AH8" s="33"/>
       <c r="AI8" s="17"/>
       <c r="AJ8" s="40"/>
@@ -4921,36 +5013,36 @@
         <v>6</v>
       </c>
       <c r="C9" s="23"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="26"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="86"/>
       <c r="R9" s="33"/>
       <c r="S9" s="17"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
+      <c r="T9" s="84"/>
+      <c r="U9" s="85"/>
+      <c r="V9" s="85"/>
+      <c r="W9" s="85"/>
+      <c r="X9" s="85"/>
+      <c r="Y9" s="86"/>
       <c r="Z9" s="33"/>
       <c r="AA9" s="17"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
+      <c r="AB9" s="76"/>
+      <c r="AC9" s="77"/>
+      <c r="AD9" s="77"/>
+      <c r="AE9" s="77"/>
+      <c r="AF9" s="77"/>
+      <c r="AG9" s="78"/>
       <c r="AH9" s="33"/>
       <c r="AI9" s="17"/>
       <c r="AJ9" s="40"/>
@@ -5041,20 +5133,24 @@
         <v>9</v>
       </c>
       <c r="C12" s="23"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="D12" s="70">
+        <v>64</v>
+      </c>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="88"/>
       <c r="J12" s="26"/>
       <c r="K12" s="23"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
+      <c r="L12" s="70">
+        <v>65</v>
+      </c>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="88"/>
       <c r="R12" s="33"/>
       <c r="S12" s="17"/>
       <c r="T12" s="23"/>
@@ -5081,24 +5177,20 @@
         <v>10</v>
       </c>
       <c r="C13" s="23"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="18"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="91"/>
       <c r="J13" s="26"/>
       <c r="K13" s="23"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="18"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="90"/>
+      <c r="P13" s="90"/>
+      <c r="Q13" s="91"/>
       <c r="R13" s="33"/>
       <c r="S13" s="17"/>
       <c r="T13" s="23"/>
@@ -5108,14 +5200,14 @@
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
       <c r="Z13" s="33"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="60"/>
-      <c r="AC13" s="60"/>
-      <c r="AD13" s="60"/>
-      <c r="AE13" s="60"/>
-      <c r="AF13" s="60"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="70"/>
+      <c r="AA13" s="95"/>
+      <c r="AB13" s="87"/>
+      <c r="AC13" s="87"/>
+      <c r="AD13" s="87"/>
+      <c r="AE13" s="87"/>
+      <c r="AF13" s="87"/>
+      <c r="AG13" s="87"/>
+      <c r="AH13" s="96"/>
       <c r="AI13" s="17"/>
       <c r="AJ13" s="40"/>
     </row>
@@ -5125,20 +5217,20 @@
         <v>11</v>
       </c>
       <c r="C14" s="23"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="18"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="91"/>
       <c r="J14" s="26"/>
       <c r="K14" s="23"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="18"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="91"/>
       <c r="R14" s="33"/>
       <c r="S14" s="17"/>
       <c r="T14" s="23"/>
@@ -5148,14 +5240,14 @@
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
       <c r="Z14" s="33"/>
-      <c r="AA14" s="71"/>
-      <c r="AB14" s="63"/>
-      <c r="AC14" s="63"/>
-      <c r="AD14" s="63"/>
-      <c r="AE14" s="63"/>
-      <c r="AF14" s="63"/>
-      <c r="AG14" s="63"/>
-      <c r="AH14" s="72"/>
+      <c r="AA14" s="97"/>
+      <c r="AB14" s="90"/>
+      <c r="AC14" s="90"/>
+      <c r="AD14" s="90"/>
+      <c r="AE14" s="90"/>
+      <c r="AF14" s="90"/>
+      <c r="AG14" s="90"/>
+      <c r="AH14" s="98"/>
       <c r="AI14" s="17"/>
       <c r="AJ14" s="40"/>
     </row>
@@ -5165,20 +5257,20 @@
         <v>12</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="18"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="91"/>
       <c r="J15" s="26"/>
       <c r="K15" s="23"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="18"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="91"/>
       <c r="R15" s="33"/>
       <c r="S15" s="17"/>
       <c r="T15" s="23"/>
@@ -5188,14 +5280,14 @@
       <c r="X15" s="18"/>
       <c r="Y15" s="18"/>
       <c r="Z15" s="33"/>
-      <c r="AA15" s="71"/>
-      <c r="AB15" s="63"/>
-      <c r="AC15" s="63"/>
-      <c r="AD15" s="63"/>
-      <c r="AE15" s="63"/>
-      <c r="AF15" s="63"/>
-      <c r="AG15" s="63"/>
-      <c r="AH15" s="72"/>
+      <c r="AA15" s="97"/>
+      <c r="AB15" s="90"/>
+      <c r="AC15" s="90"/>
+      <c r="AD15" s="90"/>
+      <c r="AE15" s="90"/>
+      <c r="AF15" s="90"/>
+      <c r="AG15" s="90"/>
+      <c r="AH15" s="98"/>
       <c r="AI15" s="17"/>
       <c r="AJ15" s="40"/>
     </row>
@@ -5205,20 +5297,20 @@
         <v>13</v>
       </c>
       <c r="C16" s="23"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="18"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="91"/>
       <c r="J16" s="26"/>
       <c r="K16" s="23"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="18"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="91"/>
       <c r="R16" s="33"/>
       <c r="S16" s="17"/>
       <c r="T16" s="23"/>
@@ -5228,14 +5320,14 @@
       <c r="X16" s="18"/>
       <c r="Y16" s="18"/>
       <c r="Z16" s="33"/>
-      <c r="AA16" s="73"/>
-      <c r="AB16" s="66"/>
-      <c r="AC16" s="66"/>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="66"/>
-      <c r="AG16" s="66"/>
-      <c r="AH16" s="74"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="93"/>
+      <c r="AE16" s="93"/>
+      <c r="AF16" s="93"/>
+      <c r="AG16" s="93"/>
+      <c r="AH16" s="100"/>
       <c r="AI16" s="17"/>
       <c r="AJ16" s="40"/>
     </row>
@@ -5245,20 +5337,20 @@
         <v>14</v>
       </c>
       <c r="C17" s="23"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94"/>
       <c r="J17" s="26"/>
       <c r="K17" s="23"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="94"/>
       <c r="R17" s="33"/>
       <c r="S17" s="17"/>
       <c r="T17" s="23"/>
@@ -5439,13 +5531,14 @@
       <c r="AK21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="AA13:AH16"/>
-    <mergeCell ref="E5:H8"/>
-    <mergeCell ref="M5:P8"/>
-    <mergeCell ref="U5:X8"/>
-    <mergeCell ref="E13:H16"/>
-    <mergeCell ref="M13:P16"/>
+    <mergeCell ref="D4:I9"/>
+    <mergeCell ref="L4:Q9"/>
+    <mergeCell ref="T4:Y9"/>
+    <mergeCell ref="AB4:AG9"/>
+    <mergeCell ref="L12:Q17"/>
+    <mergeCell ref="D12:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>